<commit_message>
Added in Druid skills doc 5 new skills. Druid skills doc finished!
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Done/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
+++ b/GameDesign/Class/Done/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
   </bookViews>
   <sheets>
     <sheet name="1-ProtectiveWings" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -1431,7 +1431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2316,7 +2316,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>